<commit_message>
output files from most recent sprint
</commit_message>
<xml_diff>
--- a/SESAR/trainingDataApproach/output/materialSampleType-10ep-.0001-20batch-100kSamKaggle.xlsx
+++ b/SESAR/trainingDataApproach/output/materialSampleType-10ep-.0001-20batch-100kSamKaggle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944a82e2ddcde9eb/Documents/GithubC/iSamples/content-classification/SESAR/output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944a82e2ddcde9eb/Documents/GithubC/iSamples/content-classification/SESAR/trainingDataApproach/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="7" documentId="8_{9F348732-76EC-4DB9-B82B-78DED35C4013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FC11DA6-4063-46CC-BAAC-5BCFE5DBEC47}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1170" windowWidth="11955" windowHeight="14880" xr2:uid="{70EEA1A9-5780-474F-8676-3247A8B4B6B1}"/>
+    <workbookView xWindow="1350" yWindow="5460" windowWidth="17040" windowHeight="9990" xr2:uid="{70EEA1A9-5780-474F-8676-3247A8B4B6B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,6 +172,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533C7803-2C59-4237-A483-764C098AD536}">
   <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>